<commit_message>
Start per female fecundity script
</commit_message>
<xml_diff>
--- a/original/Early_Experience_Original.xlsx
+++ b/original/Early_Experience_Original.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngomae/MyGithub/early_experience/data/original/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngomae/MyGithub/early_experience/original/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9648D77A-7CA6-3244-9F34-7DF66191A0C5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5257F3C-50F9-6646-80A9-671E4CAF6E0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4040" yWindow="1300" windowWidth="24760" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="to_print" sheetId="3" r:id="rId2"/>
     <sheet name="Diet_order" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -25,12 +25,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="39">
   <si>
     <t>collectedEggs</t>
   </si>
@@ -144,6 +150,9 @@
   </si>
   <si>
     <t>male</t>
+  </si>
+  <si>
+    <t>censored</t>
   </si>
 </sst>
 </file>
@@ -608,10 +617,10 @@
   <dimension ref="A1:N355"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F329" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D357" sqref="D357"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -655,7 +664,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>10</v>

</xml_diff>